<commit_message>
add script and plots
</commit_message>
<xml_diff>
--- a/specs_airplane.xlsx
+++ b/specs_airplane.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>Engine Type</t>
   </si>
   <si>
@@ -39,9 +36,6 @@
     <t>Falcon 200</t>
   </si>
   <si>
-    <t>G V</t>
-  </si>
-  <si>
     <t>Hawker 800</t>
   </si>
   <si>
@@ -69,18 +63,12 @@
     <t>Dassault Falcon</t>
   </si>
   <si>
-    <t>Gulfstream</t>
-  </si>
-  <si>
     <t>Hawker Beechcraft</t>
   </si>
   <si>
     <t>DA42</t>
   </si>
   <si>
-    <t>B36TC-Bonanza</t>
-  </si>
-  <si>
     <t>172SP</t>
   </si>
   <si>
@@ -96,25 +84,37 @@
     <t>Citation III</t>
   </si>
   <si>
-    <t>Cruise Speed (kts)</t>
-  </si>
-  <si>
-    <t>Gross Weight (kg)</t>
-  </si>
-  <si>
-    <t>Empty Weight (kg)</t>
-  </si>
-  <si>
-    <t>Range (nm)</t>
-  </si>
-  <si>
-    <t>Service Ceiling (m)</t>
-  </si>
-  <si>
-    <t>Max Speed (kts)</t>
-  </si>
-  <si>
-    <t>Length (m)</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>B36 Bonanza</t>
+  </si>
+  <si>
+    <t>Max Speed, kts</t>
+  </si>
+  <si>
+    <t>Cruise Speed, kts</t>
+  </si>
+  <si>
+    <t>Service Ceiling, m</t>
+  </si>
+  <si>
+    <t>Max Gross, kg</t>
+  </si>
+  <si>
+    <t>Empty Weight, kg</t>
+  </si>
+  <si>
+    <t>Range, nm</t>
+  </si>
+  <si>
+    <t>Length, m</t>
+  </si>
+  <si>
+    <t>HondaJet</t>
+  </si>
+  <si>
+    <t>Honda</t>
   </si>
 </sst>
 </file>
@@ -600,121 +600,121 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5">
         <v>211</v>
@@ -744,7 +744,7 @@
         <v>521</v>
       </c>
       <c r="K4" s="5">
-        <v>516</v>
+        <v>422</v>
       </c>
       <c r="L4" s="5">
         <v>463</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="5">
         <v>180</v>
@@ -782,7 +782,7 @@
         <v>435</v>
       </c>
       <c r="K5" s="5">
-        <v>459</v>
+        <v>368</v>
       </c>
       <c r="L5" s="5">
         <v>432</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6">
         <v>5334</v>
@@ -820,7 +820,7 @@
         <v>11887.2</v>
       </c>
       <c r="K6" s="6">
-        <v>15544.8</v>
+        <v>13106</v>
       </c>
       <c r="L6" s="6">
         <v>12496.8</v>
@@ -858,7 +858,7 @@
         <v>14514.955840000001</v>
       </c>
       <c r="K7" s="6">
-        <v>40551.157877999998</v>
+        <v>4808</v>
       </c>
       <c r="L7" s="6">
         <v>12428.430938000001</v>
@@ -896,7 +896,7 @@
         <v>8527.5365559999991</v>
       </c>
       <c r="K8" s="6">
-        <v>21228.122916</v>
+        <v>3267</v>
       </c>
       <c r="L8" s="6">
         <v>6858.3166344000001</v>
@@ -934,7 +934,7 @@
         <v>2500</v>
       </c>
       <c r="K9" s="6">
-        <v>6500</v>
+        <v>1206</v>
       </c>
       <c r="L9" s="6">
         <v>2642</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7">
         <v>7.918704</v>
@@ -972,7 +972,7 @@
         <v>17.160240000000002</v>
       </c>
       <c r="K10" s="7">
-        <v>29.2608</v>
+        <v>13</v>
       </c>
       <c r="L10" s="7">
         <v>15.5448</v>

</xml_diff>